<commit_message>
migrating to bootstrap CDN
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihailtudos/Google Drive/openClassRooms/project_4/P4-Project-Updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CBCDA6-B9D9-604C-B9BC-56A419588468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297E9131-40C3-2948-93D3-C757BFD80588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Category</t>
   </si>
@@ -69,15 +69,9 @@
     <t xml:space="preserve">Removing it but could be added at any point back. Focusing on descriptive metatags and content to help SEO and website ranking. </t>
   </si>
   <si>
-    <t>description metatag</t>
-  </si>
-  <si>
     <t>MOZ</t>
   </si>
   <si>
-    <t xml:space="preserve">The description tag is not helping in site ranking since 2009 according to Google but it is used to attract clicks when the website is searched on google. </t>
-  </si>
-  <si>
     <t>A page's meta description should intelligently (read: in a natural, active, non-spammy way) employ the keywords that page is targeting, but also create a compelling description that a searcher will want to click. It should be directly relevant to the page it describes, and unique from the descriptions for other pages.</t>
   </si>
   <si>
@@ -108,9 +102,6 @@
     <t>hiddent keywords</t>
   </si>
   <si>
-    <t>SEO/performance</t>
-  </si>
-  <si>
     <t>Blackhat techniques (hiding keyward) were used and have been removed</t>
   </si>
   <si>
@@ -120,9 +111,6 @@
     <t>Hiding text or links in your content to manipulate Google's search rankings can be seen as deceptive and is a violation of Google's Webmaster Guidelines.</t>
   </si>
   <si>
-    <t>Performance/accessibility</t>
-  </si>
-  <si>
     <t>scripts</t>
   </si>
   <si>
@@ -141,13 +129,7 @@
     <t>css and js files</t>
   </si>
   <si>
-    <t>Linked css and js files are not minified, a version would reduce the size of the curent download.</t>
-  </si>
-  <si>
     <t>replacing the current files with  minified versions of it</t>
-  </si>
-  <si>
-    <t>accessibility</t>
   </si>
   <si>
     <t>text contrast</t>
@@ -179,6 +161,27 @@
   </si>
   <si>
     <t>Web Accessibility Guidelines</t>
+  </si>
+  <si>
+    <t>metatag</t>
+  </si>
+  <si>
+    <t>The description tag is not helping in site ranking since 2009 according to Google but it is used to attract clicks when the website is searched on google, also  the keywords metatag is not usefull</t>
+  </si>
+  <si>
+    <t>Linked css and js files are not minified, a minified version would reduce the size of the curent download</t>
+  </si>
+  <si>
+    <t>SEO/Accessibility</t>
+  </si>
+  <si>
+    <t>SEO/Performance</t>
+  </si>
+  <si>
+    <t>Performance/Accessibility</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
   </si>
 </sst>
 </file>
@@ -529,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="174" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -609,139 +612,139 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="D5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="F6" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="F7" s="12" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="C9" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
reduced the fontawesome css file content
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihailtudos/Google Drive/openClassRooms/project_4/P4-Project-Updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297E9131-40C3-2948-93D3-C757BFD80588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8042089-FAFF-2046-99FC-78E05EB694C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Category</t>
   </si>
@@ -54,30 +54,12 @@
     <t xml:space="preserve">SEO </t>
   </si>
   <si>
-    <t>keyward meta tag</t>
-  </si>
-  <si>
-    <t>Google doesn't use these metatags because they can be easily coppied.</t>
-  </si>
-  <si>
-    <t>Google Search Center Blog</t>
-  </si>
-  <si>
-    <t>Removing the metatag, a paid enterprise service could be bought from google</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Removing it but could be added at any point back. Focusing on descriptive metatags and content to help SEO and website ranking. </t>
-  </si>
-  <si>
     <t>MOZ</t>
   </si>
   <si>
     <t>A page's meta description should intelligently (read: in a natural, active, non-spammy way) employ the keywords that page is targeting, but also create a compelling description that a searcher will want to click. It should be directly relevant to the page it describes, and unique from the descriptions for other pages.</t>
   </si>
   <si>
-    <t xml:space="preserve">Creating a more attractive and catchy description to attract user's clicks </t>
-  </si>
-  <si>
     <t xml:space="preserve">Accessibility/performance </t>
   </si>
   <si>
@@ -96,9 +78,6 @@
     <t>Title is missing there is only a . (dot) as the title of the page which is not SEO good practive neither a user-friendly technique</t>
   </si>
   <si>
-    <t>replacing curreent title with "GoMike Designs"</t>
-  </si>
-  <si>
     <t>hiddent keywords</t>
   </si>
   <si>
@@ -111,16 +90,10 @@
     <t>Hiding text or links in your content to manipulate Google's search rankings can be seen as deceptive and is a violation of Google's Webmaster Guidelines.</t>
   </si>
   <si>
-    <t>scripts</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scripts blocking the page from loading as they were placed in the header </t>
   </si>
   <si>
     <t>Render-blocking JavaScript and CSS scripts slow down your web pages, which is bad for a lot of reasons.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moving the scripts at the bottom of the website's body </t>
   </si>
   <si>
     <t>web.dev</t>
@@ -182,6 +155,21 @@
   </si>
   <si>
     <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Creating a more attractive and catchy description to attract user's clicks, removing keyword metatag, defininf en as the  lang in html tag</t>
+  </si>
+  <si>
+    <t>replacing curreent title with "GoMike Designs" for index page however a "Contact | GoMike Designs" was used for contacts page</t>
+  </si>
+  <si>
+    <t>Accessibility/Performance</t>
+  </si>
+  <si>
+    <t>scripts/render-blocking</t>
+  </si>
+  <si>
+    <t>Moving the scripts at the bottom of the website's body and defer-ing their load and preloading the CSS</t>
   </si>
 </sst>
 </file>
@@ -278,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,9 +289,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -530,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="174" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="174" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -587,199 +572,189 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:26" ht="119" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" ht="119" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="7" t="s">
+    <row r="4" spans="1:26" ht="136" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>12</v>
+      <c r="E4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="102" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="5" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="136" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>12</v>
+      <c r="F5" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>47</v>
+      <c r="A6" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>16</v>
+      <c r="D7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="8" t="s">
+    <row r="8" spans="1:26" ht="136" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>42</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="11"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="11"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="11"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -803,13 +778,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
+    <row r="18" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1790,17 +1759,15 @@
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{48719DB5-2B65-6641-9DCF-45F703EE0AF9}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{61682C61-4192-424C-85B9-E4433A3D983F}"/>
-    <hyperlink ref="F4" r:id="rId3" display="Google developers " xr:uid="{0EA07777-55A6-C54A-83ED-8C9D469FDE6B}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{8ABA38F0-41E5-7A40-9BAA-6AB4C9A4733B}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{9A5EC8F1-5CE4-A442-A512-F341E40EF209}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{A919112E-EBA8-2845-8B53-9200BB3797CC}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{300A6BBB-DFD9-D041-AAAC-6B8A20BE2716}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{5E0C967F-63CC-B144-93F4-1783DE8BC8F2}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{61682C61-4192-424C-85B9-E4433A3D983F}"/>
+    <hyperlink ref="F3" r:id="rId2" display="Google developers " xr:uid="{0EA07777-55A6-C54A-83ED-8C9D469FDE6B}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{8ABA38F0-41E5-7A40-9BAA-6AB4C9A4733B}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{9A5EC8F1-5CE4-A442-A512-F341E40EF209}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{A919112E-EBA8-2845-8B53-9200BB3797CC}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{300A6BBB-DFD9-D041-AAAC-6B8A20BE2716}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{5E0C967F-63CC-B144-93F4-1783DE8BC8F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
preloading font files before load to ensure text is dispalyed properly
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihailtudos/Google Drive/openClassRooms/project_4/P4-Project-Updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8042089-FAFF-2046-99FC-78E05EB694C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D874AC74-7513-A14E-B6C2-B4B55F541F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>css and js files</t>
   </si>
   <si>
-    <t>replacing the current files with  minified versions of it</t>
-  </si>
-  <si>
     <t>text contrast</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>The description tag is not helping in site ranking since 2009 according to Google but it is used to attract clicks when the website is searched on google, also  the keywords metatag is not usefull</t>
   </si>
   <si>
-    <t>Linked css and js files are not minified, a minified version would reduce the size of the curent download</t>
-  </si>
-  <si>
     <t>SEO/Accessibility</t>
   </si>
   <si>
@@ -170,6 +164,12 @@
   </si>
   <si>
     <t>Moving the scripts at the bottom of the website's body and defer-ing their load and preloading the CSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked css and js files are not minified, a minified version would reduce the size of the curent download, also there are extra css in those files which needs to be removed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">replacing the current files with  minified versions of it, also removed unused css </t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="174" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="174" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -577,16 +577,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>7</v>
@@ -600,13 +600,13 @@
         <v>22</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>10</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="4" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>12</v>
@@ -626,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>7</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="5" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>15</v>
@@ -654,10 +654,10 @@
     </row>
     <row r="6" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>19</v>
@@ -666,7 +666,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>21</v>
@@ -674,47 +674,47 @@
     </row>
     <row r="7" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>

</xml_diff>

<commit_message>
modified the excel SEO template
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihailtudos/Google Drive/openClassRooms/project_4/P4-Project-Updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D874AC74-7513-A14E-B6C2-B4B55F541F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6921079-3FE3-C24E-AC08-35BBD6FEE3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Category</t>
   </si>
@@ -75,24 +75,15 @@
     <t>A title tag is an HTML element that specifies the title of a web page. Title tags are displayed on search engine results pages (SERPs) as the clickable headline for a given result, and are important for usability, SEO, and social sharing. The title tag of a web page is meant to be an accurate and concise description of a page's content.</t>
   </si>
   <si>
-    <t>Title is missing there is only a . (dot) as the title of the page which is not SEO good practive neither a user-friendly technique</t>
-  </si>
-  <si>
     <t>hiddent keywords</t>
   </si>
   <si>
-    <t>Blackhat techniques (hiding keyward) were used and have been removed</t>
-  </si>
-  <si>
     <t>Removing all blackhat elements from the page and building content that helps highlight those keywords</t>
   </si>
   <si>
     <t>Hiding text or links in your content to manipulate Google's search rankings can be seen as deceptive and is a violation of Google's Webmaster Guidelines.</t>
   </si>
   <si>
-    <t xml:space="preserve">Scripts blocking the page from loading as they were placed in the header </t>
-  </si>
-  <si>
     <t>Render-blocking JavaScript and CSS scripts slow down your web pages, which is bad for a lot of reasons.</t>
   </si>
   <si>
@@ -105,40 +96,18 @@
     <t>text contrast</t>
   </si>
   <si>
-    <t>By using sufficiently-contrasting colors, a website's font visibility is stark enough to distinguish — meaning the great content developed for a website can be read by everyone.</t>
-  </si>
-  <si>
-    <t>The guidelines say that normal text (including images of text) must meet a contrast ratio of at least 4.5:1; large text (18 point or larger, or 14 point or larger and bold) should have a contrast ratio of at least 3:1</t>
-  </si>
-  <si>
-    <t>have created more contrast that makes text more visible and therefore easier to read</t>
-  </si>
-  <si>
     <t>Bureau of Internet Accessibility</t>
   </si>
   <si>
     <t xml:space="preserve">semantic HTML </t>
   </si>
   <si>
-    <t>Structural, semantic HTML is the key starting point toward good accessibility practices.
-When a screen reader, or any sort of assistive device scans a web page, it gets information about the HTML structure of the page and therefore giving context to your page/content</t>
-  </si>
-  <si>
-    <t>Secific HTML elements should be used to tell the browser what functional purpose your content serves. These other HTML elements provide meaning to the browser and assistive technology about what you’re saying on your website, so you should choose them based on what the content is - not based on how they look with graphics.</t>
-  </si>
-  <si>
-    <t>Have replaced meaningless elements with more meaninfull elements such as section, articale, aside, headings, etc.</t>
-  </si>
-  <si>
     <t>Web Accessibility Guidelines</t>
   </si>
   <si>
     <t>metatag</t>
   </si>
   <si>
-    <t>The description tag is not helping in site ranking since 2009 according to Google but it is used to attract clicks when the website is searched on google, also  the keywords metatag is not usefull</t>
-  </si>
-  <si>
     <t>SEO/Accessibility</t>
   </si>
   <si>
@@ -151,25 +120,89 @@
     <t>Accessibility</t>
   </si>
   <si>
-    <t>Creating a more attractive and catchy description to attract user's clicks, removing keyword metatag, defininf en as the  lang in html tag</t>
-  </si>
-  <si>
-    <t>replacing curreent title with "GoMike Designs" for index page however a "Contact | GoMike Designs" was used for contacts page</t>
-  </si>
-  <si>
     <t>Accessibility/Performance</t>
   </si>
   <si>
     <t>scripts/render-blocking</t>
   </si>
   <si>
-    <t>Moving the scripts at the bottom of the website's body and defer-ing their load and preloading the CSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linked css and js files are not minified, a minified version would reduce the size of the curent download, also there are extra css in those files which needs to be removed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">replacing the current files with  minified versions of it, also removed unused css </t>
+    <t xml:space="preserve">sitemap </t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lazy load iamges </t>
+  </si>
+  <si>
+    <t>Lazy-loading is a technique that defers loading of non-critical resources at page load time. Instead, these non-critical resources are loaded at the moment of need. Where images are concerned, "non-critical" is often synonymous with "off-screen"</t>
+  </si>
+  <si>
+    <t>The description tag is not helping in site ranking since 2009, according to Google. However, it is used to attract clicks when the website is searched on google, also the keywords metatag is not any useful anymore.</t>
+  </si>
+  <si>
+    <t>Creating a more attractive and catchy description to attract user's clicks. 
+Removing keyword metatag. 
+Defininf en as the  lang in html tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linked css and js files are not minified, a minified version would reduce the size of the current download, also there are extra css in those files which needs to be removed. </t>
+  </si>
+  <si>
+    <t>Replaced the current files with minified versions of it, also removed unused css where possible.</t>
+  </si>
+  <si>
+    <t>Title is missing, there is only a . (dot) as the title of the page which is not SEO good practice neither a user-friendly technique.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replaced current title with "GoMike Designs" for home page and a "Contact | GoMike Designs" content was used for the contacts page. </t>
+  </si>
+  <si>
+    <t>Blackhat techniques (hiding keyword) were used and have been removed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scripts blocking the page from loading as they were placed in the header and therefore would require time to load before the rest of the content is loaded.  </t>
+  </si>
+  <si>
+    <t>Moving the scripts at the bottom of the website's body and defer-ing their load. 
+ Preloading the CSS</t>
+  </si>
+  <si>
+    <t>The guidelines say that normal text (including images of text) must meet a contrast ratio of at least 4.5:1; large text (18 point or larger, or 14 point or larger and bold) should have a contrast ratio of at least 3:1. 
+By using sufficiently-contrasting colors, a website's font visibility is stark enough to distinguish — meaning the great content developed for a website can be read by everyone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are may instances where the text is not readable due to the contrast of font size. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have created more contrast that makes text more visible and therefore easier to read. 
+Increased the font size where required and also added line-height where required. </t>
+  </si>
+  <si>
+    <t>Secific HTML elements should be used to tell the browser what functional purpose your content serves. These other HTML elements provide meaning to the browser and assistive technology about what you’re saying on your website, so you should choose them based on what the content is - not based on how they look with graphics.
+Structural, semantic HTML is the key starting point toward good accessibility practices.
+When a screen reader, or any sort of assistive device scans a web page, it gets information about the HTML structure of the page and therefore gives context to your page/content.</t>
+  </si>
+  <si>
+    <t>The whole website is semantically incorrectly structured as there were only used generic tags such as div, p, span, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have replaced meaningless elements (generic elements) with more meaningful tags such as section, article, aside, headings, etc. which gives the page more context. </t>
+  </si>
+  <si>
+    <t>There is no sitemap link on the website or sitemap file generated for the website.</t>
+  </si>
+  <si>
+    <t>Search engines like Google read this file to crawl your site more efficiently. A sitemap tells Google which pages and files you think are important in your site, and also provides valuable information about these files. But also helps impaired users.</t>
+  </si>
+  <si>
+    <t>Generated a sitemap.xml file and added a link at the bottom of the website.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lazy loading images which allows loading only the media content on the website at the needed time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All images are loaded at the load time hence negatively impacting the loading time. After converting the images to webp format and resizing some of them it would have a good impact if the images and media content that is not needed at the load time would be lazy loaded or not loaded at all. Therefore, improving the performance of the website. </t>
   </si>
 </sst>
 </file>
@@ -266,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +331,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -517,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="174" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="174" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -572,21 +608,21 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>39</v>
+      <c r="E2" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>7</v>
@@ -597,16 +633,16 @@
         <v>9</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>10</v>
@@ -614,13 +650,13 @@
     </row>
     <row r="4" spans="1:26" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>13</v>
@@ -634,100 +670,123 @@
     </row>
     <row r="5" spans="1:26" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>43</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="187" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="6" t="s">
+    <row r="8" spans="1:26" ht="272" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="8" spans="1:26" ht="136" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="6" t="s">
+    <row r="9" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="C9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="170" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
@@ -1768,6 +1827,8 @@
     <hyperlink ref="F6" r:id="rId5" xr:uid="{A919112E-EBA8-2845-8B53-9200BB3797CC}"/>
     <hyperlink ref="F7" r:id="rId6" xr:uid="{300A6BBB-DFD9-D041-AAAC-6B8A20BE2716}"/>
     <hyperlink ref="F8" r:id="rId7" xr:uid="{5E0C967F-63CC-B144-93F4-1783DE8BC8F2}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{495878FC-587A-1946-BBE1-E78F3B424F3E}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{36D2C38E-E1B1-524C-8F9D-08266A5B3D85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
added padding to modal-dialog images
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihailtudos/Google Drive/openClassRooms/project_4/P4-Project-Updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6921079-3FE3-C24E-AC08-35BBD6FEE3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24B3A11-5ECB-1945-8909-28A3310C3EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Category</t>
   </si>
@@ -203,6 +203,21 @@
   </si>
   <si>
     <t xml:space="preserve">All images are loaded at the load time hence negatively impacting the loading time. After converting the images to webp format and resizing some of them it would have a good impact if the images and media content that is not needed at the load time would be lazy loaded or not loaded at all. Therefore, improving the performance of the website. </t>
+  </si>
+  <si>
+    <t>custom image size</t>
+  </si>
+  <si>
+    <t>The same image size would be loaded for the mobile and desktop version of the website which impacts directly the preformance especially on mobiles as the users on mobiles don't need large media content</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Loading the most appropriate image for the viewer's display would help in saving bandwidth and speeding page load times.</t>
+  </si>
+  <si>
+    <t>Have added different image sizes for mobile and desktop versions of the website.</t>
+  </si>
+  <si>
+    <t>MDN</t>
   </si>
 </sst>
 </file>
@@ -553,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="174" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="174" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -788,12 +803,25 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="6"/>
+    <row r="11" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
@@ -1829,6 +1857,7 @@
     <hyperlink ref="F8" r:id="rId7" xr:uid="{5E0C967F-63CC-B144-93F4-1783DE8BC8F2}"/>
     <hyperlink ref="F9" r:id="rId8" xr:uid="{495878FC-587A-1946-BBE1-E78F3B424F3E}"/>
     <hyperlink ref="F10" r:id="rId9" xr:uid="{36D2C38E-E1B1-524C-8F9D-08266A5B3D85}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{90DD7D7C-20DF-4845-9A41-501924678119}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>